<commit_message>
Include all parameters with a valid value
</commit_message>
<xml_diff>
--- a/message_ix/genie_tech/tech_data.xlsx
+++ b/message_ix/genie_tech/tech_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pratama\Documents\GitHub\MESSAGEix\message_ix\message_ix\genie_tech\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64840B77-FBE6-4BED-98F3-2FCAC6FDE1F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF8B3216-4DE3-4BB0-A956-5383A6B01445}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2652" yWindow="2652" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
   <si>
     <t>inv_cost</t>
   </si>
@@ -39,9 +39,6 @@
     <t>fix_cost</t>
   </si>
   <si>
-    <t>emissions_factor</t>
-  </si>
-  <si>
     <t>input</t>
   </si>
   <si>
@@ -127,6 +124,24 @@
   </si>
   <si>
     <t>year</t>
+  </si>
+  <si>
+    <t>emission_factor</t>
+  </si>
+  <si>
+    <t>output</t>
+  </si>
+  <si>
+    <t>commodity_out</t>
+  </si>
+  <si>
+    <t>level_out</t>
+  </si>
+  <si>
+    <t>light</t>
+  </si>
+  <si>
+    <t>useful</t>
   </si>
 </sst>
 </file>
@@ -445,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -460,10 +475,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
         <v>21</v>
-      </c>
-      <c r="C1" t="s">
-        <v>22</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -471,175 +486,193 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
         <v>15</v>
-      </c>
-      <c r="D6" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" t="s">
         <v>26</v>
-      </c>
-      <c r="C7" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8">
-        <v>2500</v>
+        <v>16</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9">
-        <v>100</v>
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10">
-        <v>10</v>
+        <v>35</v>
+      </c>
+      <c r="D10" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="D11" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" t="s">
-        <v>20</v>
+        <v>0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12">
+        <v>2500</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" t="s">
+        <v>23</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C14" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D14">
-        <v>-20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16">
-        <v>20</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="B17" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C17" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D17">
-        <v>0.5</v>
+        <v>-20</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21">
         <v>0.5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Initialise learning input automation
</commit_message>
<xml_diff>
--- a/message_ix/genie_tech/tech_data.xlsx
+++ b/message_ix/genie_tech/tech_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pratama\Documents\GitHub\MESSAGEix\message_ix\message_ix\genie_tech\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{161F3E36-D6A4-4187-842E-F8FB2BA3ED65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{499FC1B5-53C4-4B09-81EE-D85300A2722D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
   <si>
     <t>inv_cost</t>
   </si>
@@ -144,23 +144,54 @@
     <t>useful</t>
   </si>
   <si>
-    <t>learning_rate</t>
-  </si>
-  <si>
-    <t>eos_rate</t>
-  </si>
-  <si>
     <t>technology</t>
+  </si>
+  <si>
+    <t>learning_par</t>
+  </si>
+  <si>
+    <t>eos_par</t>
+  </si>
+  <si>
+    <t>wind_ppl</t>
+  </si>
+  <si>
+    <t>nbr_unit_ref</t>
+  </si>
+  <si>
+    <t>u_ref</t>
+  </si>
+  <si>
+    <t>size</t>
+  </si>
+  <si>
+    <t>small,medium,large</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>5,10,50</t>
+  </si>
+  <si>
+    <t>technology,size</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -186,9 +217,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -469,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -482,7 +514,7 @@
     <col min="4" max="4" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>20</v>
       </c>
@@ -492,8 +524,11 @@
       <c r="D1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -501,19 +536,19 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -521,7 +556,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -529,7 +564,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -537,7 +572,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -545,7 +580,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -553,7 +588,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>35</v>
       </c>
@@ -561,7 +596,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -569,7 +604,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -583,7 +618,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -597,7 +632,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -611,17 +646,17 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -635,7 +670,7 @@
         <v>-20</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -646,7 +681,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -660,7 +695,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -674,7 +709,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -685,23 +720,80 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" t="s">
         <v>39</v>
       </c>
-      <c r="B22" t="s">
+      <c r="E22">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>40</v>
-      </c>
       <c r="B23" t="s">
-        <v>41</v>
+        <v>39</v>
+      </c>
+      <c r="E23">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E24">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>44</v>
+      </c>
+      <c r="B25" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>45</v>
+      </c>
+      <c r="E26" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27" t="s">
+        <v>49</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E27" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed adding learning parameters
</commit_message>
<xml_diff>
--- a/message_ix/genie_tech/tech_data.xlsx
+++ b/message_ix/genie_tech/tech_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pratama\Documents\GitHub\MESSAGEix\message_ix\message_ix\genie_tech\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{499FC1B5-53C4-4B09-81EE-D85300A2722D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDC4660A-4959-45A8-8716-5E819886EBDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -504,7 +504,7 @@
   <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -650,10 +650,16 @@
       <c r="A15" t="s">
         <v>4</v>
       </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>34</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Migrating to use yaml data format
</commit_message>
<xml_diff>
--- a/message_ix/genie_tech/tech_data.xlsx
+++ b/message_ix/genie_tech/tech_data.xlsx
@@ -8,12 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pratama\Documents\GitHub\MESSAGEix\message_ix\message_ix\genie_tech\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDC4660A-4959-45A8-8716-5E819886EBDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F40E06-5688-4D8D-B5B4-FCFC309B6F23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="DACCS_pars" sheetId="2" r:id="rId2"/>
+    <sheet name="DACCS_sets" sheetId="3" r:id="rId3"/>
+    <sheet name="DACCS_region" sheetId="4" r:id="rId4"/>
+    <sheet name="DACCS_time" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="62">
   <si>
     <t>inv_cost</t>
   </si>
@@ -175,6 +179,42 @@
   </si>
   <si>
     <t>technology,size</t>
+  </si>
+  <si>
+    <t>par</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>DACCS_LT</t>
+  </si>
+  <si>
+    <t>set</t>
+  </si>
+  <si>
+    <t>first_active_year</t>
+  </si>
+  <si>
+    <t>region</t>
+  </si>
+  <si>
+    <t>NAM</t>
+  </si>
+  <si>
+    <t>WEU</t>
+  </si>
+  <si>
+    <t>inv_cost_reduction_rate</t>
+  </si>
+  <si>
+    <t>% / yr</t>
+  </si>
+  <si>
+    <t>fraction</t>
   </si>
 </sst>
 </file>
@@ -503,8 +543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -802,4 +842,377 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{244E55F5-937A-43BB-A622-3CB0A117AB8A}">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11">
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCF5B0C5-5CF8-4D5F-A002-6849E9585E28}">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9">
+        <v>2020</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA55F9F2-782B-458A-98C3-E2D8EFAD28C7}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3">
+        <v>1.2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C31DA6B0-D877-426A-9489-7D3D973FECEC}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2">
+        <v>0.05</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>